<commit_message>
Fix parser. Add unit-test. Fix EA table
</commit_message>
<xml_diff>
--- a/Конечный автомат парсера.xlsx
+++ b/Конечный автомат парсера.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton_Tsel\IdeaProjects\myProjects\LinerCalculator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8181E35-B997-4B3B-BB7D-98DC18C43C38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="20400" windowHeight="8265" activeTab="1"/>
+    <workbookView xWindow="3195" yWindow="1800" windowWidth="20910" windowHeight="11835" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ver1" sheetId="1" r:id="rId1"/>
@@ -150,7 +156,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -631,7 +637,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -639,14 +645,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -684,9 +693,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -719,9 +728,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -754,9 +780,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -929,7 +972,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -938,9 +981,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="9.625" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
-    <col min="12" max="12" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1430,17 +1473,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="49.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="56.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1825,7 +1868,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>